<commit_message>
tree of db-add name
</commit_message>
<xml_diff>
--- a/data/apprentice_PROD_4.xlsx
+++ b/data/apprentice_PROD_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OZKL\T_H\backflask---T.H-app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DD9822-F5D4-45B0-90F0-E380F618F123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6E3DD3E-282F-4E4D-805B-06A043633060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,16 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet 1'!$A$1:$AZ$6</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="MyGCk/QkN/mZDsNtthXwkORa67ayIQoVqSodSDAjRGs="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="125">
   <si>
     <t>שם</t>
   </si>
@@ -391,6 +386,18 @@
   </si>
   <si>
     <t>חגי</t>
+  </si>
+  <si>
+    <t>ערד</t>
+  </si>
+  <si>
+    <t>אלעד</t>
+  </si>
+  <si>
+    <t>ספק</t>
+  </si>
+  <si>
+    <t>עלי</t>
   </si>
 </sst>
 </file>
@@ -470,13 +477,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="6"/>
-      <color rgb="FF212121"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,6 +506,12 @@
       <patternFill patternType="solid">
         <fgColor theme="2"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4CCCC"/>
+        <bgColor rgb="FFF4CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -526,11 +539,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -569,11 +583,20 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{B0E2F804-6F90-4879-A236-A2DCA4C87E3C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -788,8 +811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -1000,8 +1023,8 @@
       <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="20">
-        <v>504083796</v>
+      <c r="C2" s="21">
+        <v>528827064</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>53</v>
@@ -1148,7 +1171,7 @@
         <v>108</v>
       </c>
       <c r="AZ2" s="20">
-        <v>504083795</v>
+        <v>528827064</v>
       </c>
     </row>
     <row r="3" spans="1:53" ht="24" customHeight="1">
@@ -1158,11 +1181,11 @@
       <c r="B3" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="20">
-        <v>504083797</v>
+      <c r="C3" s="22">
+        <v>528827065</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>53</v>
+        <v>121</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>54</v>
@@ -1304,7 +1327,7 @@
         <v>108</v>
       </c>
       <c r="AZ3" s="20">
-        <v>504083795</v>
+        <v>528827064</v>
       </c>
     </row>
     <row r="4" spans="1:53" ht="15.5">
@@ -1314,8 +1337,8 @@
       <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="20">
-        <v>504083798</v>
+      <c r="C4" s="22">
+        <v>528827066</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>53</v>
@@ -1363,7 +1386,7 @@
         <v>65</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="T4" s="6" t="s">
         <v>67</v>
@@ -1375,7 +1398,7 @@
         <v>68</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
       <c r="X4" s="6" t="s">
         <v>67</v>
@@ -1402,7 +1425,7 @@
         <v>544816497</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG4" s="5">
         <v>544816497</v>
@@ -1423,7 +1446,7 @@
         <v>544816497</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="AN4" s="2" t="s">
         <v>75</v>
@@ -1462,7 +1485,7 @@
         <v>108</v>
       </c>
       <c r="AZ4" s="20">
-        <v>504083795</v>
+        <v>528827064</v>
       </c>
     </row>
     <row r="5" spans="1:53" ht="15.5">
@@ -1472,11 +1495,11 @@
       <c r="B5" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="20">
-        <v>504083799</v>
+      <c r="C5" s="22">
+        <v>528827067</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>54</v>
@@ -1620,7 +1643,7 @@
         <v>108</v>
       </c>
       <c r="AZ5" s="20">
-        <v>504083795</v>
+        <v>528827064</v>
       </c>
     </row>
     <row r="6" spans="1:53" ht="15.5">
@@ -1630,8 +1653,8 @@
       <c r="B6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C6" s="20">
-        <v>504083800</v>
+      <c r="C6" s="22">
+        <v>528827068</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>53</v>
@@ -1778,7 +1801,7 @@
         <v>108</v>
       </c>
       <c r="AZ6" s="20">
-        <v>504083795</v>
+        <v>528827064</v>
       </c>
     </row>
     <row r="7" spans="1:53" ht="15.5">

</xml_diff>